<commit_message>
Actualización con mejoras de extracción
</commit_message>
<xml_diff>
--- a/web-automation-framework/src/main/resources/excel/data1.xlsx
+++ b/web-automation-framework/src/main/resources/excel/data1.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView windowHeight="2760" windowWidth="14670" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="DATA" r:id="rId1" sheetId="1"/>
+    <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,114 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>DATA</t>
   </si>
   <si>
     <t>TC</t>
-  </si>
-  <si>
-    <t>123900000023120
-123900000023121
-123900000023122
-123900000023123
-123900000023124
-123900000023125
-123900000023126
-123900000023127
-123900000023128
-123900000023129
-123900000023130
-123900000023131
-123900000023132
-123900000023133
-123900000023134
-123900000023135
-123900000023136
-123900000023137
-123900000023138
-123900000023139
-123900000023140
-123900000023141
-123900000023142
-123900000023143
-123900000023144
-123900000023145
-123900000023146
-123900000023147
-123900000023148
-123900000023149
-123900000023150
-123900000023151
-123900000023152
-123900000023153
-123900000023154
-123900000023155
-123900000023156
-123900000023157
-123900000023158
-123900000023159
-123900000023160
-123900000023161
-123900000023162
-123900000023163
-123900000023164
-123900000023165
-123900000023166
-123900000023167
-123900000023168
-123900000023169
-123900000023170
-123900000023171
-123900000023172
-123900000023173
-123900000023174
-123900000023175
-123900000023176
-123900000023177
-123900000023178
-123900000023179
-123900000023180
-123900000023181
-123900000023182
-123900000023183
-123900000023184
-123900000023185
-123900000023186
-123900000023187
-123900000023188
-123900000023189
-123900000023190
-123900000023191
-123900000023192
-123900000023193
-123900000023194
-123900000023195
-123900000023196
-123900000023197
-123900000023198
-123900000023199
-123900000023200
-123900000023201
-123900000023202
-123900000023203
-123900000023204
-123900000023205
-123900000023206
-123900000023207
-123900000023208
-123900000023209
-123900000023210
-123900000023211
-123900000023212
-123900000023213
-123900000023214
-123900000023215
-123900000023216
-123900000023217
-123900000023218
-123900000023219</t>
   </si>
   <si>
     <t>123900000023220
@@ -1077,72 +975,116 @@
     <t>RESULTADOS (TC10)</t>
   </si>
   <si>
-    <t>123900000023120</t>
-  </si>
-  <si>
-    <t>123900000023138</t>
-  </si>
-  <si>
-    <t>123900000023146</t>
-  </si>
-  <si>
-    <t>123900000023153</t>
-  </si>
-  <si>
-    <t>123900000023161</t>
-  </si>
-  <si>
-    <t>123900000023179</t>
-  </si>
-  <si>
-    <t>123900000023187</t>
-  </si>
-  <si>
-    <t>123900000023195</t>
-  </si>
-  <si>
-    <t>123900000023203</t>
-  </si>
-  <si>
-    <t>123900000023211</t>
-  </si>
-  <si>
-    <t>123900000023229</t>
-  </si>
-  <si>
-    <t>123900000023237</t>
-  </si>
-  <si>
-    <t>123900000023245</t>
-  </si>
-  <si>
-    <t>123900000023252</t>
-  </si>
-  <si>
-    <t>123900000023260</t>
-  </si>
-  <si>
-    <t>123900000023278</t>
-  </si>
-  <si>
-    <t>123900000023286</t>
-  </si>
-  <si>
-    <t>123900000023294</t>
-  </si>
-  <si>
-    <t>123900000023302</t>
-  </si>
-  <si>
-    <t>123900000023310</t>
+    <t/>
+  </si>
+  <si>
+    <t>123900000130181
+123900000130182
+123900000130183
+123900000130184
+123900000130185
+123900000130186
+123900000130187
+123900000130188
+123900000130189
+123900000130190
+123900000130191
+123900000130192
+123900000130193
+123900000130194
+123900000130195
+123900000130196
+123900000130197
+123900000130198
+123900000130199
+123900000130200
+123900000130201
+123900000130202
+123900000130203
+123900000130204
+123900000130205
+123900000130206
+123900000130207
+123900000130208
+123900000130209
+123900000130210
+123900000130211
+123900000130212
+123900000130213
+123900000130214
+123900000130215
+123900000130216
+123900000130217
+123900000130218
+123900000130219
+123900000130220
+123900000130221
+123900000130222
+123900000130223
+123900000130224
+123900000130225
+123900000130226
+123900000130227
+123900000130228
+123900000130229
+123900000130230
+123900000130231
+123900000130232
+123900000130233
+123900000130234
+123900000130235
+123900000130236
+123900000130237
+123900000130238
+123900000130239
+123900000130240
+123900000130241
+123900000130242
+123900000130243
+123900000130244
+123900000130245
+123900000130246
+123900000130247
+123900000130248
+123900000130249
+123900000130250
+123900000130251
+123900000130252
+123900000130253
+123900000130254
+123900000130255
+123900000130256
+123900000130257
+123900000130258
+123900000130259
+123900000130260
+123900000130261
+123900000130262
+123900000130263
+123900000130264
+123900000130265
+123900000130266
+123900000130267
+123900000130268
+123900000130269
+123900000130270
+123900000130271
+123900000130272
+123900000130273
+123900000130274
+123900000130275
+123900000130276
+123900000130277
+123900000130278
+123900000130279
+123900000130280</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1165,106 +1107,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1284,47 +1126,27 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1341,10 +1163,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1379,7 +1201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1414,7 +1236,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1508,21 +1330,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1539,7 +1361,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1591,27 +1413,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="D2" sqref="D2:E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="4" max="13" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="13" width="22.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1620,238 +1442,280 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="2" s="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="3" s="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="4" s="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="5" s="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="6" s="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="7" s="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="8" s="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="9" s="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="10" s="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>40</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="11" s="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" t="s">
-        <v>41</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15" r="12" s="1" spans="1:13" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" customHeight="1" ht="15" r="13" s="1" spans="1:13" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" customHeight="1" ht="15" r="14" s="1" spans="1:13" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="15" s="1" spans="1:13" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="16" s="1" spans="1:13" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="17" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="18" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="19" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="20" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="21" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="22" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="23" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="24" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="25" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="26" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="27" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="28" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="29" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="30" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="31" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="32" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="33" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="34" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="35" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="36" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="37" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="38" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="39" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="40" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="41" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="42" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="43" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="44" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="45" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="46" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="47" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="48" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="49" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="50" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="51" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="52" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="53" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="54" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="55" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="56" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="57" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="58" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="59" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="60" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="61" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="62" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="63" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="64" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="65" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="66" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="67" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="68" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="69" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="70" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="71" s="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>